<commit_message>
Arrumei o win32, adicionei os comandos e o pyperclip
</commit_message>
<xml_diff>
--- a/16.01.0001.xlsx
+++ b/16.01.0001.xlsx
@@ -1,43 +1,102 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Downloads\Projects\Projetos\Python\Excel_Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18144ACA-D3CD-4F6B-968C-1260EACEAD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Value" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Value" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>TITULO</t>
+  </si>
+  <si>
+    <t>SERIE</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>MOTIVO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>PREÇO</t>
+  </si>
+  <si>
+    <t>BANCO</t>
+  </si>
+  <si>
+    <t>12121</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>Cancelamento</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>7780</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -100,95 +159,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -476,122 +474,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="14.5703125" customWidth="1" min="1" max="1"/>
-    <col width="21.5703125" customWidth="1" min="2" max="2"/>
-    <col width="10.140625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>CPF</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>NOME</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>TITULO</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>SERIE</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>MOTIVO</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>TIPO</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>PREÇO</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>BANCO</t>
-        </is>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>666.666.666-12</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Roberto Carlos Da Silva</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>12121</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
-        <is>
-          <t>AG</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="F2" s="5" t="inlineStr">
-        <is>
-          <t>Cancelamento</t>
-        </is>
-      </c>
-      <c r="G2" s="6" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="H2" s="8" t="n">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6">
         <v>400</v>
       </c>
-      <c r="I2" s="6" t="inlineStr">
-        <is>
-          <t>7780</t>
-        </is>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="C4" s="4" t="n"/>
-      <c r="D4" s="4" t="n"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6">
-      <c r="H6" s="4" t="n"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
26/03/2025 0.5:  Dei suporte a todas as libs, código está funcional porém está dando um "erro" no terminal sempre que utilizo starto a func
</commit_message>
<xml_diff>
--- a/16.01.0001.xlsx
+++ b/16.01.0001.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Downloads\Projects\Projetos\Python\Excel_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18144ACA-D3CD-4F6B-968C-1260EACEAD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C958C207-2293-43F5-A81F-E0C308579664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>TITULO</t>
   </si>
@@ -43,40 +43,34 @@
     <t>BANCO</t>
   </si>
   <si>
-    <t>12121</t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>Cancelamento</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>7780</t>
-  </si>
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Idade</t>
-  </si>
-  <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>Maria</t>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>EMISSAO</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>RESPONSAVEL</t>
+  </si>
+  <si>
+    <t>000.000.000-12</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Requirement already satisfied: keyboard in c:\users\olive\appdata\local\programs\python\python313\lib\site-packages (0.13.5)_x000D_
+_x000D_
+[notice] A new release of pip is available: 24.3.1 -&gt; 25.0.1_x000D_
+[notice] To update, run: C:\Users\olive\AppData\Local\Programs\Python\Python313\python.exe -m pip install --upgrade pip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,12 +161,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,93 +476,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3">
-        <v>30</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="6">
-        <v>400</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H6" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
23/04/2025 | | 	- Substitui win32com.client por uma lib menos pesada e menos bugada. 	- Lib nova e funcional (Até agora) xlwings funciona tanto com o excel aberto e com o excel em segundo plano, perfeito para Análise de Dados
</commit_message>
<xml_diff>
--- a/16.01.0001.xlsx
+++ b/16.01.0001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Downloads\Projects\Projetos\Python\Excel_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C958C207-2293-43F5-A81F-E0C308579664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69739BA8-773A-4BF9-B2C0-8A3B131A5334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TITULO</t>
   </si>
@@ -55,22 +55,19 @@
     <t>RESPONSAVEL</t>
   </si>
   <si>
-    <t>000.000.000-12</t>
-  </si>
-  <si>
-    <t>José</t>
-  </si>
-  <si>
-    <t>Requirement already satisfied: keyboard in c:\users\olive\appdata\local\programs\python\python313\lib\site-packages (0.13.5)_x000D_
-_x000D_
-[notice] A new release of pip is available: 24.3.1 -&gt; 25.0.1_x000D_
-[notice] To update, run: C:\Users\olive\AppData\Local\Programs\Python\Python313\python.exe -m pip install --upgrade pip</t>
+    <t>josé</t>
+  </si>
+  <si>
+    <t>100.100.100-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,10 +165,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -478,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +487,7 @@
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
     <col min="10" max="11" width="10.28515625" customWidth="1"/>
@@ -533,34 +530,32 @@
     </row>
     <row r="2" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="7"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -573,7 +568,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -584,9 +579,9 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -599,7 +594,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -612,7 +607,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -622,10 +617,10 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="7"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -638,7 +633,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -651,7 +646,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="J10" s="7"/>
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -664,7 +659,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="J11" s="7"/>
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -677,7 +672,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -690,7 +685,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -703,7 +698,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -716,7 +711,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="7"/>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -729,7 +724,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -742,7 +737,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="7"/>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -755,7 +750,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="J18" s="7"/>
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -768,7 +763,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -781,7 +776,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="J20" s="7"/>
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -794,7 +789,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="7"/>
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -807,7 +802,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="J22" s="7"/>
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
24/04/2025 | Existe .exe para execução. readerMe com notas a fazer pois á formas de melhorar a experiência do usúario
</commit_message>
<xml_diff>
--- a/16.01.0001.xlsx
+++ b/16.01.0001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Downloads\Projects\Projetos\Python\Excel_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69739BA8-773A-4BF9-B2C0-8A3B131A5334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF80217-BD04-4348-97BA-7ED2DB5FA8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>TITULO</t>
   </si>
@@ -59,6 +59,21 @@
   </si>
   <si>
     <t>100.100.100-01</t>
+  </si>
+  <si>
+    <t>ricardo williands</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>11/00/1</t>
+  </si>
+  <si>
+    <t>Cancelamento</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -150,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,6 +185,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,20 +553,38 @@
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5">
+        <v>54102</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="7">
+        <v>50</v>
+      </c>
+      <c r="K2" s="5">
+        <v>2379</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="6"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>

</xml_diff>

<commit_message>
Feito uma fomar de pesquisar o arquivo antes de excutar o script 13/05/2025
</commit_message>
<xml_diff>
--- a/16.01.0001.xlsx
+++ b/16.01.0001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Downloads\Projects\Projetos\Python\Excel_Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF80217-BD04-4348-97BA-7ED2DB5FA8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0B9432-CC56-4F56-B53C-E5AA49CD7960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1110" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>TITULO</t>
   </si>
@@ -55,25 +55,13 @@
     <t>RESPONSAVEL</t>
   </si>
   <si>
-    <t>josé</t>
-  </si>
-  <si>
-    <t>100.100.100-01</t>
-  </si>
-  <si>
-    <t>ricardo williands</t>
-  </si>
-  <si>
-    <t>AH</t>
-  </si>
-  <si>
-    <t>11/00/1</t>
-  </si>
-  <si>
-    <t>Cancelamento</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>José</t>
+  </si>
+  <si>
+    <t>300.000.003-12</t>
+  </si>
+  <si>
+    <t>ricardo foda</t>
   </si>
 </sst>
 </file>
@@ -493,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,30 +544,14 @@
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5">
-        <v>54102</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="7">
-        <v>50</v>
-      </c>
-      <c r="K2" s="5">
-        <v>2379</v>
-      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>

</xml_diff>